<commit_message>
fixing bugs related to reading candidates from CDF
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data/test_set_0_skipped_first_choice/test_set_0_skipped_first_choice_cvr.xlsx
+++ b/src/test/resources/test_data/test_set_0_skipped_first_choice/test_set_0_skipped_first_choice_cvr.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10403"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggilber\Documents\RCV Project\BrightSpots\RCV Test Data Consolidated\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leisenberg/code/rcv/src/test/resources/test_data/test_set_0_skipped_first_choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DD12F5-8B9B-C94D-870F-E1CC4C77CABD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22540" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="11">
   <si>
     <t>Ballot #</t>
   </si>
@@ -57,15 +58,12 @@
   </si>
   <si>
     <t>overvote</t>
-  </si>
-  <si>
-    <t>TestSet0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -634,19 +632,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="5" width="13.42578125" customWidth="1"/>
+    <col min="2" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -663,7 +661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -680,7 +678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -697,7 +695,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -714,7 +712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -731,7 +729,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -748,7 +746,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -765,7 +763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -782,7 +780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -799,7 +797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -816,7 +814,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -833,7 +831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -850,7 +848,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -867,12 +865,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-    </row>
+    <row r="14" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>